<commit_message>
Fixed Address to pass UT as well as corresponding; UTVolAddress bug fixes
</commit_message>
<xml_diff>
--- a/UT.Vol.BLL/HelperFiles/VolAddress.xlsx
+++ b/UT.Vol.BLL/HelperFiles/VolAddress.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -67,9 +67,6 @@
     <t>AZ</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('1','1700 W. Washington','','','Phoenix','AZ','85007','','1')</t>
-  </si>
-  <si>
     <t>820 N. French St.</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>DE</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('2','820 N. French St.','','','Wilmington','DE','19801','','0')</t>
-  </si>
-  <si>
     <t>700 W. Jefferson</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('3','700 W. Jefferson','','','Boise','ID','83720','','1')</t>
-  </si>
-  <si>
     <t>700 Capitol Ave.</t>
   </si>
   <si>
@@ -103,9 +94,6 @@
     <t>KY</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('4','700 Capitol Ave.','','','Frankfurt','KY','40601','','1')</t>
-  </si>
-  <si>
     <t>75 Constitution Ave.</t>
   </si>
   <si>
@@ -115,9 +103,6 @@
     <t>MN</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('5','75 Constitution Ave.','','','St. Paul','MN','55155','','0')</t>
-  </si>
-  <si>
     <t>101 N. Carson Street</t>
   </si>
   <si>
@@ -127,9 +112,6 @@
     <t>NV</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('6','101 N. Carson Street','','','Carson City','NV','89701','','1')</t>
-  </si>
-  <si>
     <t>116 West Jones St.</t>
   </si>
   <si>
@@ -139,9 +121,6 @@
     <t>NC</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('7','116 West Jones St.','','','Raleigh','NC','27603','','0')</t>
-  </si>
-  <si>
     <t>600 E. Boulevard Avenue</t>
   </si>
   <si>
@@ -151,9 +130,6 @@
     <t>ND</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('8','600 E. Boulevard Avenue','','','Bismark','ND','58505','','0')</t>
-  </si>
-  <si>
     <t>225 Main Capitol</t>
   </si>
   <si>
@@ -163,9 +139,6 @@
     <t>PA</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('9','225 Main Capitol','','','Harrisburg','PA','17120','','0')</t>
-  </si>
-  <si>
     <t>109 State St.</t>
   </si>
   <si>
@@ -175,9 +148,6 @@
     <t>VT</t>
   </si>
   <si>
-    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('10','109 State St.','','','Montpelier','VT','56409','','0')</t>
-  </si>
-  <si>
     <t>dba53101-f9b2-4dc0-85e7-11d472fd99cd</t>
   </si>
   <si>
@@ -212,13 +182,43 @@
   </si>
   <si>
     <t>PrimaryAddr</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('1','1700 W. Washington','','','Phoenix','AZ','85007', NULL,'1')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('2','820 N. French St.','','','Wilmington','DE','19801', NULL,'0')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('3','700 W. Jefferson','','','Boise','ID','83720',NULL,'1')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('4','700 Capitol Ave.','','','Frankfurt','KY','40601',NULL,'1')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('5','75 Constitution Ave.','','','St. Paul','MN','55155',NULL,'0')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('6','101 N. Carson Street','','','Carson City','NV','89701',NULL,'1')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('7','116 West Jones St.','','','Raleigh','NC','27603',NULL,'0')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('8','600 E. Boulevard Avenue','','','Bismark','ND','58505',NULL,'0')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('9','225 Main Capitol','','','Harrisburg','PA','17120',NULL,'0')</t>
+  </si>
+  <si>
+    <t>INSERT INTO [VolTeer].[Vol].[tblVolAddress] (AddrID,AddrLine1,AddrLine2,AddrLine3,City,St,Zip,Zip4,ActiveFlg) VALUES('10','109 State St.','','','Montpelier','VT','56409',NULL,'0')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -351,7 +351,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -386,7 +385,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -562,14 +560,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.7109375"/>
     <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
@@ -589,12 +587,12 @@
     <col min="16" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -624,7 +622,7 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
@@ -636,12 +634,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -669,30 +667,30 @@
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
-        <v>17</v>
+      <c r="O2" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="2">
         <v>19801</v>
@@ -706,30 +704,30 @@
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2" t="s">
-        <v>21</v>
+      <c r="O3" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I4" s="2">
         <v>83720</v>
@@ -743,30 +741,30 @@
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="2" t="s">
-        <v>25</v>
+      <c r="O4" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I5" s="2">
         <v>40601</v>
@@ -780,30 +778,30 @@
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2" t="s">
-        <v>29</v>
+      <c r="O5" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2">
         <v>55155</v>
@@ -817,30 +815,30 @@
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="2" t="s">
-        <v>33</v>
+      <c r="O6" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2">
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I7" s="2">
         <v>89701</v>
@@ -854,30 +852,30 @@
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="2" t="s">
-        <v>37</v>
+      <c r="O7" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="I8" s="2">
         <v>27603</v>
@@ -891,30 +889,30 @@
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="2" t="s">
-        <v>41</v>
+      <c r="O8" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I9" s="2">
         <v>58505</v>
@@ -928,30 +926,30 @@
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="2" t="s">
-        <v>45</v>
+      <c r="O9" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2">
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I10" s="2">
         <v>17120</v>
@@ -965,30 +963,30 @@
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="2" t="s">
-        <v>49</v>
+      <c r="O10" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="I11" s="2">
         <v>56409</v>
@@ -1002,8 +1000,8 @@
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="2" t="s">
-        <v>53</v>
+      <c r="O11" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>